<commit_message>
Author               : Prateek Kapoor File Modified        : Product Backlog.xlsx Description          : Added search by SCGJ Batch number in view documents
</commit_message>
<xml_diff>
--- a/Requirements/Product Backlog/Product Backlog.xlsx
+++ b/Requirements/Product Backlog/Product Backlog.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashmi kapoor\Desktop\NSKFDC APP\trunk\Requirements\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E087894-2AE2-41B8-91AF-79477D25D9C6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1A271022-4B5A-44B1-9046-988B7A55088D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="3345" xr2:uid="{BE25E7B5-23B0-4D7D-8D78-B63294565AEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,9 +60,6 @@
     <t>As a Product Owner, I want front end validations on username and password fields of the login page</t>
   </si>
   <si>
-    <t>As a Product Owner, I want that no unauthorise user can enter the application so that only valid user enters the application</t>
-  </si>
-  <si>
     <t>Dashboard</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t>As a Product Owner, I want the format of pdf to be generated from the system to be specified so that it can be generated from the system</t>
   </si>
   <si>
-    <t>As a Product Owner, I want a generate report button so that when I have uploaded the photographs and I click on the generate button, the report is generated and downloaded</t>
-  </si>
-  <si>
     <t>Screen</t>
   </si>
   <si>
@@ -360,9 +354,6 @@
     <t>As a Product Owner, I want static as well as user selected values for questions in the FAQ section so that I can modify the questions as per my needs</t>
   </si>
   <si>
-    <t>As a Product Owner, I want a search document functionality so that when I enter name of training partner and its batch ID and click on submit button, I can view a zip file which contains all the files uploaded by the training partner for that batch id</t>
-  </si>
-  <si>
     <t>As a Product Owner, I want when I click on the zip icon of the result, the file should be downloaded so that, I can view the files uploaded by the training partner</t>
   </si>
   <si>
@@ -427,6 +418,15 @@
   </si>
   <si>
     <t>Owner</t>
+  </si>
+  <si>
+    <t>As a Product Owner, I want a show password icon along the password field so that, when I click on it the password can be seen</t>
+  </si>
+  <si>
+    <t>As a Product Owner, I want a generate report button so that when I have uploaded the photographs and I click on the generate button, the report is generated and downloaded in zip file</t>
+  </si>
+  <si>
+    <t>As a Product Owner, I want a search document functionality so that when I enter name of training partner and its batch ID or SCGJ Batch Number and click on submit button, I can view a zip file which contains all the files uploaded by the training partner for that batch id</t>
   </si>
 </sst>
 </file>
@@ -605,14 +605,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -623,41 +626,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC5FB69-8FB6-4AB0-A622-325661F11E81}">
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50:Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,102 +995,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
       <c r="R3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>8</v>
@@ -1112,11 +1112,11 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>9</v>
@@ -1138,11 +1138,11 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>10</v>
@@ -1164,14 +1164,14 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -1190,204 +1190,204 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
+        <v>29</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
       <c r="R8" s="2"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="20"/>
+      <c r="B9" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="22"/>
       <c r="E9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
+        <v>30</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
+        <v>31</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
+        <v>32</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
+        <v>33</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
+        <v>35</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -1406,40 +1406,40 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
+        <v>37</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
@@ -1458,14 +1458,14 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
@@ -1484,14 +1484,14 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -1510,14 +1510,14 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -1536,14 +1536,14 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -1562,14 +1562,14 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -1588,14 +1588,14 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -1614,14 +1614,14 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -1640,18 +1640,18 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
-      <c r="B25" s="16" t="s">
-        <v>21</v>
+      <c r="B25" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -1670,14 +1670,14 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
-      <c r="B26" s="16"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="23"/>
       <c r="D26" s="23"/>
       <c r="E26" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -1696,14 +1696,14 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
-      <c r="B27" s="16"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="23"/>
       <c r="D27" s="23"/>
       <c r="E27" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -1722,40 +1722,40 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
-      <c r="B28" s="16"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="23"/>
       <c r="D28" s="23"/>
       <c r="E28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
+        <v>49</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
-      <c r="B29" s="16"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="23"/>
       <c r="D29" s="23"/>
       <c r="E29" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -1774,14 +1774,14 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="B30" s="16"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
       <c r="E30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
@@ -1800,14 +1800,14 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="B31" s="16"/>
+      <c r="B31" s="18"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
@@ -1826,14 +1826,14 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
-      <c r="B32" s="16"/>
+      <c r="B32" s="18"/>
       <c r="C32" s="23"/>
       <c r="D32" s="23"/>
       <c r="E32" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
@@ -1852,18 +1852,18 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="24"/>
+      <c r="B33" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="21"/>
       <c r="E33" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
@@ -1882,14 +1882,14 @@
     </row>
     <row r="34" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
       <c r="E34" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
@@ -1908,40 +1908,40 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
       <c r="E35" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
+        <v>79</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
     <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
@@ -1960,72 +1960,72 @@
     </row>
     <row r="37" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
       <c r="E37" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
+        <v>83</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
     <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
       <c r="E38" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
+        <v>84</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
     <row r="39" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
@@ -2044,14 +2044,14 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
@@ -2070,122 +2070,122 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
+        <v>95</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
       <c r="E43" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
+        <v>96</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
+        <v>97</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
     <row r="45" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
-      <c r="B45" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="D45" s="26"/>
+      <c r="B45" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="17"/>
       <c r="E45" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -2204,14 +2204,14 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
       <c r="E46" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
@@ -2230,14 +2230,14 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
       <c r="E47" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
@@ -2256,26 +2256,26 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
       <c r="E48" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
+        <v>101</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
@@ -2283,17 +2283,17 @@
     <row r="49" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C49" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="27"/>
+        <v>127</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="10"/>
       <c r="E49" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -2313,25 +2313,25 @@
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
+        <v>118</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
@@ -2339,25 +2339,25 @@
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="9"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
       <c r="E51" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F51" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="17"/>
-      <c r="L51" s="17"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="17"/>
-      <c r="O51" s="17"/>
-      <c r="P51" s="17"/>
-      <c r="Q51" s="17"/>
+        <v>119</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
@@ -2365,17 +2365,17 @@
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D52" s="21"/>
+        <v>128</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="13"/>
       <c r="E52" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
@@ -2395,13 +2395,13 @@
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="9"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
       <c r="E53" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -2421,13 +2421,13 @@
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="9"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
       <c r="E54" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
@@ -2447,13 +2447,13 @@
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="9"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
       <c r="E55" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
@@ -2473,13 +2473,13 @@
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="9"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -2499,13 +2499,13 @@
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="9"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
       <c r="E57" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
@@ -2525,25 +2525,25 @@
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="9"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
       <c r="E58" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F58" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
-      <c r="K58" s="13"/>
-      <c r="L58" s="13"/>
-      <c r="M58" s="13"/>
-      <c r="N58" s="13"/>
-      <c r="O58" s="13"/>
-      <c r="P58" s="13"/>
-      <c r="Q58" s="13"/>
+        <v>126</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="14"/>
+      <c r="P58" s="14"/>
+      <c r="Q58" s="14"/>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
       <c r="T58" s="3" t="e">
@@ -2583,41 +2583,33 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="F6:Q6"/>
+    <mergeCell ref="F8:Q8"/>
+    <mergeCell ref="C4:D8"/>
     <mergeCell ref="A1:T2"/>
     <mergeCell ref="F3:Q3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F4:Q4"/>
     <mergeCell ref="F5:Q5"/>
-    <mergeCell ref="F7:Q7"/>
-    <mergeCell ref="F9:Q9"/>
-    <mergeCell ref="F6:Q6"/>
-    <mergeCell ref="F8:Q8"/>
-    <mergeCell ref="C4:D8"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="F13:Q13"/>
-    <mergeCell ref="F14:Q14"/>
+    <mergeCell ref="A4:A38"/>
     <mergeCell ref="F10:Q10"/>
     <mergeCell ref="F11:Q11"/>
     <mergeCell ref="F12:Q12"/>
-    <mergeCell ref="F16:Q16"/>
-    <mergeCell ref="F19:Q19"/>
-    <mergeCell ref="F20:Q20"/>
-    <mergeCell ref="F21:Q21"/>
-    <mergeCell ref="F33:Q33"/>
+    <mergeCell ref="F7:Q7"/>
+    <mergeCell ref="F9:Q9"/>
+    <mergeCell ref="F32:Q32"/>
+    <mergeCell ref="F26:Q26"/>
+    <mergeCell ref="F31:Q31"/>
+    <mergeCell ref="F24:Q24"/>
+    <mergeCell ref="F13:Q13"/>
+    <mergeCell ref="F14:Q14"/>
     <mergeCell ref="F25:Q25"/>
     <mergeCell ref="F27:Q27"/>
     <mergeCell ref="F28:Q28"/>
     <mergeCell ref="F29:Q29"/>
     <mergeCell ref="F30:Q30"/>
-    <mergeCell ref="F32:Q32"/>
-    <mergeCell ref="F26:Q26"/>
-    <mergeCell ref="F31:Q31"/>
-    <mergeCell ref="F24:Q24"/>
-    <mergeCell ref="F34:Q34"/>
-    <mergeCell ref="F35:Q35"/>
-    <mergeCell ref="F36:Q36"/>
-    <mergeCell ref="F37:Q37"/>
-    <mergeCell ref="F38:Q38"/>
+    <mergeCell ref="C33:D38"/>
     <mergeCell ref="B33:B38"/>
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="C9:D14"/>
@@ -2625,14 +2617,6 @@
     <mergeCell ref="C25:D32"/>
     <mergeCell ref="B15:B24"/>
     <mergeCell ref="C15:D24"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="F50:Q50"/>
-    <mergeCell ref="F51:Q51"/>
-    <mergeCell ref="F15:Q15"/>
-    <mergeCell ref="F17:Q17"/>
-    <mergeCell ref="F18:Q18"/>
-    <mergeCell ref="F23:Q23"/>
-    <mergeCell ref="F22:Q22"/>
     <mergeCell ref="B39:B44"/>
     <mergeCell ref="C39:D44"/>
     <mergeCell ref="F39:Q39"/>
@@ -2640,12 +2624,27 @@
     <mergeCell ref="F41:Q41"/>
     <mergeCell ref="F44:Q44"/>
     <mergeCell ref="F42:Q42"/>
-    <mergeCell ref="C33:D38"/>
-    <mergeCell ref="F46:Q46"/>
-    <mergeCell ref="F47:Q47"/>
+    <mergeCell ref="F51:Q51"/>
+    <mergeCell ref="F15:Q15"/>
+    <mergeCell ref="F17:Q17"/>
+    <mergeCell ref="F18:Q18"/>
+    <mergeCell ref="F23:Q23"/>
+    <mergeCell ref="F22:Q22"/>
+    <mergeCell ref="F34:Q34"/>
+    <mergeCell ref="F35:Q35"/>
+    <mergeCell ref="F36:Q36"/>
+    <mergeCell ref="F37:Q37"/>
+    <mergeCell ref="F38:Q38"/>
+    <mergeCell ref="F16:Q16"/>
+    <mergeCell ref="F19:Q19"/>
+    <mergeCell ref="F20:Q20"/>
+    <mergeCell ref="F21:Q21"/>
+    <mergeCell ref="F33:Q33"/>
     <mergeCell ref="F48:Q48"/>
     <mergeCell ref="F49:Q49"/>
     <mergeCell ref="C45:D48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="F50:Q50"/>
     <mergeCell ref="A39:A58"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="B52:B58"/>
@@ -2658,9 +2657,10 @@
     <mergeCell ref="F57:Q57"/>
     <mergeCell ref="C52:D58"/>
     <mergeCell ref="F58:Q58"/>
-    <mergeCell ref="A4:A38"/>
     <mergeCell ref="F45:Q45"/>
     <mergeCell ref="F43:Q43"/>
+    <mergeCell ref="F46:Q46"/>
+    <mergeCell ref="F47:Q47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>